<commit_message>
Add Day 5 spreadsheet
</commit_message>
<xml_diff>
--- a/Day4/Day4Workings.xlsx
+++ b/Day4/Day4Workings.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalyfalero/Documents/Programming/AoC2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natalyfalero/Documents/Programming/AoC2020/AoC2020Excel/Day4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0241D3-77CC-A14C-8457-0ED0218739B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3702073F-F3A7-A84E-8368-2EAE04E177D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="980" windowWidth="27640" windowHeight="16060" xr2:uid="{F031F079-F073-2040-A95F-D31DF7DC7932}"/>
   </bookViews>
@@ -2426,7 +2426,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2436,6 +2436,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2753,26 +2756,48 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BC1141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AM3" sqref="AM3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="67.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="75.83203125" customWidth="1"/>
-    <col min="25" max="25" width="10.83203125" style="3"/>
+    <col min="7" max="7" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="73.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="74" bestFit="1" customWidth="1"/>
+    <col min="18" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10.83203125" style="3"/>
-    <col min="37" max="37" width="10.83203125" style="8"/>
-    <col min="38" max="38" width="10.83203125" style="7"/>
-    <col min="39" max="39" width="10.83203125" style="8"/>
-    <col min="41" max="41" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="51" width="15.1640625" style="6" customWidth="1"/>
-    <col min="52" max="54" width="15.1640625" customWidth="1"/>
+    <col min="34" max="34" width="8" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8" style="8" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="45" max="50" width="12.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="5.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.1640625" customWidth="1"/>
+    <col min="54" max="55" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" x14ac:dyDescent="0.2">
@@ -2790,11 +2815,11 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:P2" si="0">H2+1</f>
+        <f>H2+1</f>
         <v>2</v>
       </c>
       <c r="J2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I2:P2" si="0">I2+1</f>
         <v>3</v>
       </c>
       <c r="K2">
@@ -2968,7 +2993,7 @@
         <v/>
       </c>
       <c r="O3" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(IFERROR(VLOOKUP($G3&amp;"-"&amp;O$2,$A:$B,2,FALSE),0)=0,"",VLOOKUP($G3&amp;"-"&amp;O$2,$A:$B,2,FALSE))</f>
         <v/>
       </c>
       <c r="P3" t="str">
@@ -60278,35 +60303,35 @@
         <f t="shared" si="154"/>
         <v>2</v>
       </c>
-      <c r="AG289" s="3">
+      <c r="AG289" s="5">
         <f t="shared" ref="AG289:AN289" si="180">COUNTIF(AG3:AG288,TRUE)</f>
         <v>186</v>
       </c>
-      <c r="AH289">
+      <c r="AH289" s="9">
         <f t="shared" si="180"/>
         <v>243</v>
       </c>
-      <c r="AI289">
+      <c r="AI289" s="9">
         <f t="shared" si="180"/>
         <v>238</v>
       </c>
-      <c r="AJ289">
+      <c r="AJ289" s="9">
         <f t="shared" si="180"/>
         <v>239</v>
       </c>
-      <c r="AK289" s="8">
+      <c r="AK289" s="10">
         <f t="shared" si="180"/>
         <v>243</v>
       </c>
-      <c r="AL289" s="7">
+      <c r="AL289" s="11">
         <f t="shared" si="180"/>
         <v>249</v>
       </c>
-      <c r="AM289" s="8">
+      <c r="AM289" s="10">
         <f t="shared" si="180"/>
         <v>239</v>
       </c>
-      <c r="AN289">
+      <c r="AN289" s="9">
         <f t="shared" si="180"/>
         <v>239</v>
       </c>

</xml_diff>